<commit_message>
Download file is corrected but still missing the Progress bar or some spinner to show backend processing
</commit_message>
<xml_diff>
--- a/Donwnloded/ContriesInfo.xlsx
+++ b/Donwnloded/ContriesInfo.xlsx
@@ -14,11 +14,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <x:si>
     <x:t>Benildo Mabunda DEV Challenge</x:t>
   </x:si>
   <x:si>
+    <x:t>callingCodes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>currencies</x:t>
+  </x:si>
+  <x:si>
+    <x:t>languages</x:t>
+  </x:si>
+  <x:si>
     <x:t>Nome</x:t>
   </x:si>
   <x:si>
@@ -31,9 +40,6 @@
     <x:t>alpha3Code</x:t>
   </x:si>
   <x:si>
-    <x:t>callingCodes</x:t>
-  </x:si>
-  <x:si>
     <x:t>capital</x:t>
   </x:si>
   <x:si>
@@ -70,10 +76,25 @@
     <x:t>numericCode</x:t>
   </x:si>
   <x:si>
-    <x:t>currencies</x:t>
-  </x:si>
-  <x:si>
-    <x:t>languages</x:t>
+    <x:t>code</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Symbol</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISO369_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ISO369_2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>native name</x:t>
   </x:si>
   <x:si>
     <x:t>gini</x:t>
@@ -82,18 +103,16 @@
     <x:t>translations</x:t>
   </x:si>
   <x:si>
-    <x:t>cioc</x:t>
-  </x:si>
-  <x:si>
     <x:t>regionalBlocs</x:t>
   </x:si>
   <x:si>
+    <x:t>Timeone</x:t>
+  </x:si>
+  <x:si>
     <x:t>Mozambique</x:t>
   </x:si>
   <x:si>
-    <x:t>[
-  ".mz"
-]</x:t>
+    <x:t xml:space="preserve">[.mz] </x:t>
   </x:si>
   <x:si>
     <x:t>MZ</x:t>
@@ -102,9 +121,7 @@
     <x:t>MOZ</x:t>
   </x:si>
   <x:si>
-    <x:t>[
-  "258"
-]</x:t>
+    <x:t xml:space="preserve">[258] </x:t>
   </x:si>
   <x:si>
     <x:t>Maputo</x:t>
@@ -122,79 +139,40 @@
     <x:t>https://flagcdn.com/mz.svg</x:t>
   </x:si>
   <x:si>
-    <x:t>[
-  -18.25,
-  35.0
-]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[
-  "MZ",
-  "Republic of Mozambique",
-  "República de Moçambique"
-]</x:t>
+    <x:t>Lat=-18.25, Lon=35</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">[MZ] [Republic of Mozambique] [República de Moçambique] </x:t>
   </x:si>
   <x:si>
     <x:t>Mozambican</x:t>
   </x:si>
   <x:si>
-    <x:t>[
-  "MWI",
-  "ZAF",
-  "SWZ",
-  "TZA",
-  "ZMB",
-  "ZWE"
-]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[
-  {
-    "code": "MZN",
-    "name": "Mozambican metical",
-    "symbol": "MT"
-  }
-]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[
-  {
-    "iso639_1": "pt",
-    "iso639_2": "por",
-    "name": "Portuguese",
-    "nativeName": "Português"
-  }
-]</x:t>
-  </x:si>
-  <x:si>
-    <x:t>{
-  "br": "Moçambique",
-  "pt": "Moçambique",
-  "nl": "Mozambique",
-  "hr": "Mozambik",
-  "fa": "موزامبیک",
-  "de": "Mosambik",
-  "es": "Mozambique",
-  "fr": "Mozambique",
-  "ja": "モザンビーク",
-  "it": "Mozambico",
-  "hu": "Mozambik"
-}</x:t>
-  </x:si>
-  <x:si>
-    <x:t>[
-  {
-    "acronym": "AU",
-    "name": "African Union",
-    "otherNames": [
-      "الاتحاد الأفريقي",
-      "Union africaine",
-      "União Africana",
-      "Unión Africana",
-      "Umoja wa Afrika"
-    ]
-  }
-]</x:t>
+    <x:t xml:space="preserve">[MWI] [ZAF] [SWZ] [TZA] [ZMB] [ZWE] </x:t>
+  </x:si>
+  <x:si>
+    <x:t>MZN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mozambican metical</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>pt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>por</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Portuguese</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Português</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">[UTC+02:00] </x:t>
   </x:si>
 </x:sst>
 </file>
@@ -204,7 +182,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="1">
+  <x:fonts count="2">
     <x:font>
       <x:vertAlign val="baseline"/>
       <x:sz val="11"/>
@@ -212,13 +190,31 @@
       <x:name val="Calibri"/>
       <x:family val="2"/>
     </x:font>
+    <x:font>
+      <x:b/>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="16"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="4">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FF9ACD32"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFF2003C"/>
+      </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="1">
@@ -240,18 +236,35 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="4">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
@@ -549,162 +562,222 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:X5"/>
+  <x:dimension ref="A1:AC6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="2" spans="1:24">
-      <x:c r="B2" s="0" t="s">
+    <x:row r="2" spans="1:29">
+      <x:c r="B2" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="C2" s="1" t="s"/>
+      <x:c r="D2" s="1" t="s"/>
+      <x:c r="E2" s="1" t="s"/>
+      <x:c r="F2" s="1" t="s"/>
+      <x:c r="G2" s="1" t="s"/>
+      <x:c r="H2" s="1" t="s"/>
+      <x:c r="I2" s="1" t="s"/>
+      <x:c r="J2" s="1" t="s"/>
+      <x:c r="K2" s="1" t="s"/>
+      <x:c r="L2" s="1" t="s"/>
+      <x:c r="M2" s="1" t="s"/>
+      <x:c r="N2" s="1" t="s"/>
+      <x:c r="O2" s="1" t="s"/>
+      <x:c r="P2" s="1" t="s"/>
+      <x:c r="Q2" s="1" t="s"/>
+      <x:c r="R2" s="1" t="s"/>
+      <x:c r="S2" s="1" t="s"/>
+      <x:c r="T2" s="1" t="s"/>
+      <x:c r="U2" s="1" t="s"/>
+      <x:c r="V2" s="1" t="s"/>
+      <x:c r="W2" s="1" t="s"/>
     </x:row>
-    <x:row r="4" spans="1:24">
-      <x:c r="B4" s="0" t="s">
+    <x:row r="4" spans="1:29">
+      <x:c r="F4" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C4" s="0" t="s">
+      <x:c r="S4" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D4" s="0" t="s">
+      <x:c r="T4" s="2" t="s"/>
+      <x:c r="U4" s="2" t="s"/>
+      <x:c r="V4" s="3" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="s">
+      <x:c r="W4" s="3" t="s"/>
+      <x:c r="X4" s="3" t="s"/>
+      <x:c r="Y4" s="3" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:29">
+      <x:c r="B5" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F4" s="0" t="s">
+      <x:c r="C5" s="0" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G4" s="0" t="s">
+      <x:c r="D5" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H4" s="0" t="s">
+      <x:c r="E5" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I4" s="0" t="s">
+      <x:c r="G5" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J4" s="0" t="s">
+      <x:c r="H5" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="K4" s="0" t="s">
+      <x:c r="I5" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="L4" s="0" t="s">
+      <x:c r="J5" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="M4" s="0" t="s">
+      <x:c r="K5" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="N4" s="0" t="s">
+      <x:c r="L5" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="O4" s="0" t="s">
+      <x:c r="M5" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="P4" s="0" t="s">
+      <x:c r="N5" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="Q4" s="0" t="s">
+      <x:c r="O5" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="R4" s="0" t="s">
+      <x:c r="P5" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="S4" s="0" t="s">
+      <x:c r="Q5" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="T4" s="0" t="s">
+      <x:c r="R5" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="U4" s="0" t="s">
+      <x:c r="S5" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="V4" s="0" t="s">
+      <x:c r="T5" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="W4" s="0" t="s">
+      <x:c r="U5" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="X4" s="0" t="s">
+      <x:c r="V5" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
+      <x:c r="W5" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="X5" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="Y5" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="Z5" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="AA5" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="AB5" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="AC5" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
     </x:row>
-    <x:row r="5" spans="1:24">
-      <x:c r="B5" s="0" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="C5" s="1" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="E5" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="F5" s="1" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="I5" s="0" t="s">
+    <x:row r="6" spans="1:29">
+      <x:c r="B6" s="0" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="J5" s="0" t="n">
+      <x:c r="C6" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="n">
         <x:v>31255435</x:v>
       </x:c>
-      <x:c r="K5" s="0" t="n">
+      <x:c r="K6" s="0" t="n">
         <x:v>801590</x:v>
       </x:c>
-      <x:c r="L5" s="0" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="M5" s="0" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="N5" s="1" t="s">
-        <x:v>34</x:v>
-      </x:c>
-      <x:c r="O5" s="1" t="s">
-        <x:v>35</x:v>
-      </x:c>
-      <x:c r="P5" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="Q5" s="1" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="R5" s="0" t="n">
+      <x:c r="L6" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="M6" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="N6" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="O6" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="P6" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="Q6" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="R6" s="0" t="n">
         <x:v>508</x:v>
       </x:c>
-      <x:c r="S5" s="1" t="s">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="T5" s="1" t="s">
-        <x:v>39</x:v>
-      </x:c>
-      <x:c r="U5" s="0" t="n">
+      <x:c r="S6" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="T6" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="U6" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="V6" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="W6" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="X6" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="Y6" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="Z6" s="0" t="n">
         <x:v>54</x:v>
       </x:c>
-      <x:c r="V5" s="1" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="W5" s="1" t="s">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="X5" s="0" t="s">
-        <x:v>27</x:v>
+      <x:c r="AC6" s="0" t="s">
+        <x:v>52</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
-  <x:mergeCells count="1">
+  <x:mergeCells count="3">
     <x:mergeCell ref="B2:W2"/>
+    <x:mergeCell ref="S4:U4"/>
+    <x:mergeCell ref="V4:Y4"/>
   </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>